<commit_message>
feat: update foreach/endrow/endloop with new behaviour
</commit_message>
<xml_diff>
--- a/tests/integration/data/Renderer005-ForEach-simple/expected.xlsx
+++ b/tests/integration/data/Renderer005-ForEach-simple/expected.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24580" windowHeight="14620"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24580" windowHeight="14620"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
@@ -521,22 +521,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.35" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" defaultColWidth="8.83203125"/>
   <cols>
-    <col min="1" max="1" width="5.6328125" customWidth="1"/>
-    <col min="2" max="2" width="26.08984375" customWidth="1"/>
-    <col min="3" max="4" width="7.6328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" customWidth="1"/>
+    <col min="3" max="4" width="7.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.90625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="60.08984375" customWidth="1"/>
-    <col min="8" max="8" width="5.1796875" customWidth="1"/>
-    <col min="9" max="10" width="9.08984375" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="60.1640625" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" customWidth="1"/>
+    <col min="9" max="10" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -554,7 +554,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
@@ -574,7 +574,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -594,7 +594,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -614,7 +614,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -634,7 +634,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>18</v>
       </c>
@@ -654,7 +654,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -674,7 +674,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>21</v>
       </c>

</xml_diff>